<commit_message>
Get daily reddit data: Tue Jul 30 08:09:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3406 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1efnvnh</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Natural nail visible from one side under acrylics</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx34t5dc6mfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1efnvcm</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>been seeing a lot of chappell roan sets lately…</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl3kr2086mfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1efn9mx</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Ombré gel with cat eye tips</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjpxbu3lylfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1efmpeg</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efmpeg/nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1efmlq3</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Hozier Inspired Nails!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efmlq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1efmqa2</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Shade decision??</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2l36yzu5slfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1efm6dk</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>does anyone know the cause of these chips/breakages and how to prevent them?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efm6dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1eeuad2</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>HELP… I hate my nails. How to fix?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32e5xxpu3ffd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1efmaot</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>these almost looked good until I messed with solid nail gel for the charms😩😭💀</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efmaot</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1efkyxg</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Cute emo set I did a while back ❤️✨</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efkyxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1efl4bw</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I prevent cuticle flooding while working with acrylic and poly gel ? </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efl4bw/how_do_i_prevent_cuticle_flooding_while_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1eflaai</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Spider-Man nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eflaai</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1eflero</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Short, almond, simple golden tips</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eflero</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1efg4sl</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tea bag fix on already polished nail </t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efg4sl/tea_bag_fix_on_already_polished_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1efht9b</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own nails at home </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqshmg3cekfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1efl32q</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Like third time doing press on nails🤷‍♀️🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efl32q</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1efl2we</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Cracks on multiple toe nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uax3i8cb9lfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1efl0m6</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Marble Nails😊</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf011uco8lfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1efkptv</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Y does my nail have a dent like this is this normal</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efkptv</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1efklj0</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My husband finally approved of this one</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y401xv794lfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1efk8a1</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>i’m so glad i’m (barely) able to afford getting my nails done again. it’s such a confidence boost for me. this is my favorite color i’ve gotten since i’ve started again. i’m obsessed 🩵💜</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efk8a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ef7d9b</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Damaged nails are lifting </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7d9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1efk0i7</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">greetings from chile :) read comments </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cymxk4igykfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1efjjds</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>First time trying nail tape</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efjjds/first_time_trying_nail_tape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1efjaf9</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Matched my nails to my pants 🎈</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l16kr6dkrkfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1efj7j1</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efj7j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1efizyw</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serious question, pink and white. </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9le9pbhrokfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1efirzr</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Gel polish chipping no matter what I do!!!!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/127wmrctmkfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1efimxg</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Obsessed with my new set.</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efimxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1efii2z</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Chillhouse Press on Nails Review</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efii2z/chillhouse_press_on_nails_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1efihm3</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My tech is.. amazing</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efihm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1efidpw</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>my melody 🤍🎀</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efidpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1efidab</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Help! New to gel-x manicures - Lots of growth, can't get to nail tech for another week</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efidab/help_new_to_gelx_manicures_lots_of_growth_cant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1efi9gp</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Long, Medium, Short! Oh my!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efi9gp</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1efi5iu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taking care of my nails wherever I go </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99agdweahkfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1efi4z3</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>🤍✨🫧</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt6hiwo5hkfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1efhhds</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Best overlay for natural nails?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efhhds/best_overlay_for_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1efgud2</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Me and my sisters polar opposite nails!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szpagjm06kfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1efgu9x</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cutie Pastel Frenchies </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z50syt206kfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1efgkzj</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Not sure about the dark colour</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twq8awct3kfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1efgkfp</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honestly how can I improve? </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efgkfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1efgckc</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts? </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efgckc</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1effrkc</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Gel doesn't last or work for me.. why?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1effrkc/gel_doesnt_last_or_work_for_me_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1effnv1</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>first time getting my nails done w a tech!!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1effnv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ef7cgp</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>How to reverse nail damage?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7cgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ef7z5m</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Acrylic Removal</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef7z5m/acrylic_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1efapgo</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Grainy dip?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i38pbmcouifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1efbjaf</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How Do You Protect Your Nails? </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efbjaf/how_do_you_protect_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1efeorc</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else after learning how to do nails then get them done at a salon notice how mediocre they turn out. I feel like they looked worse in person, but the first picture was right after I got them done and the shaping is so bad to me, I fixed it as much as I could when I got home. Anyone else? </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efeorc</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1eff4s4</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Nail charms...?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eff4s4/nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1eff2f5</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Attempted to do Rainbow Smoke Nails 🌈 💅🏻</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyxyx8barjfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1efezye</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Can you see those beautiful little sparkles? 😍💗</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efezye</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1efeoam</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>New nails !!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efeoam</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1efeen6</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">diy flowers </t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kty9i9xzljfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1efe48l</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New set! 🌸🩷👹</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efe48l</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1efdwsy</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with oily nails! </t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xckgah5ijfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1efd2ey</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">when you get a pedicure does the nail tech put the tools he uses in the water while he soaks your feet ? </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efd2ey/when_you_get_a_pedicure_does_the_nail_tech_put/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1efcct7</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Nail art</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efcct7/nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1efbrsc</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efbrsc/french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1efbrrd</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to remove gel polish (at a salon) and not lose your length? </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efbrrd/is_it_possible_to_remove_gel_polish_at_a_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1efblys</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Would love to hear feedback on these stained glass nail art.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efblys</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1efawbr</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efawbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1efabpm</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>just did my nails 🙈</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t28y3eb1sifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1efa2sv</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Short nails deserve love too</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms61a5iaqifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1efa2em</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Aura nails!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3odosgp7qifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1efa1uk</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my tech do me right? Flowered acrylics </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hwa4x3upifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ef9pj3</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newest set! Forgot how much I loved a good BOLD color and a sharp(ish) nail. </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef9pj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ef9k0n</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Lines on nails?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef9k0n/lines_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ef9fw1</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Is this manicure problematic enough to get a few nails redone?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef9fw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ef90g1</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>3-D Nails using regular polish!!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef90g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ef8nls</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Spooky ice cream for summer 🦇🍦</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef8nls</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ef7tpz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>PLEASE HELP!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7tpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ef7d3q</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>What design should I do?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmu45m337ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ef6nmi</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deadpool &amp; Wolverine. XD </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1243j9f02ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ef6kyh</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Client was superhappy </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he2e2lqg1ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ef6cn5</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>DIY Rubber Base</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef6cn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ef69bb</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>starry night diy</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef69bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ef604s</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>When you can see the lunula 😋🥰</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef604s</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ef5yzx</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>If you love thermals, you will love Holo Taco's I Don't Know How to Feel 5th Anniversary Collection</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef5yzx/if_you_love_thermals_you_will_love_holo_tacos_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ef5pog</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>OMG OMGG</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hscjm36dvhfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ef5jr9</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pika Pika </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahs9wbj8uhfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1eevb1o</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Primer and dehydrator making my nails pop off really easily? </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eevb1o/primer_and_dehydrator_making_my_nails_pop_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1eexrav</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>went to the nail salon for the first time in 5 years 💅🏾</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t48ftqz27gfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1eey540</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I forgot to put primer &amp; dehydrator on 4 fingers before builder gel. What’s gonna happen?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl9z0vklagfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ef4od5</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I don’t know what to ask for!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef4od5/i_dont_know_what_to_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ef4adz</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Need recommendations for water based top coat for nails in the uk</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef4adz/need_recommendations_for_water_based_top_coat_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ef3wl0</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My right hand 😭. </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9odv2gdgihfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ef3v9r</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Some mini nails that I made today, I thought they were super flirtatious</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha9rvyl6ihfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ef3s6g</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>ILNP - Carved</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs99ochkhhfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ef32ol</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Coral Chrome</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0fzgr6gchfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ef2pju</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails. First time getting ombré.. not very pleased </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzt2va1t9hfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ef2iok</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Soft gel tips with dip?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ef2iok/soft_gel_tips_with_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ef1xdp</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Tortoise French tip???</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef1xdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ef1huo</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love them!! </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef1huo</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ef1f26</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Picked a neutral base color, then told my girl she could do whatever she wanted for accent nails! </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dal3j8l0hfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ef19jw</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I think this is the nudest nude I've ever found</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f5nd85hzgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ef0ohg</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Cat eye pigment🤭</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42dog6g4vgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ef01yf</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Letting My Nails Grow: Week 8</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siwhl9diqgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ef0183</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>🪻</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvnmy7dcqgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1eeztow</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>yellow-pinkish nails🩷💖💛</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eeztow</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1efnbyr</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Glitter in the winter sun!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efnbyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1efmovc</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hozier Inspired Nails </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efmovc</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1efmobw</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Looking for alternatives to specific Lacquered Lights shades!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efmobw/looking_for_alternatives_to_specific_lacquered/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1efm2pt</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>First Ethereal Haul</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efm2pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1efk1eb</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>I Scream Nails Deal Maker 👽</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efk1eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1efhtma</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>UD Asphyxia (ca. 2000) dupe?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efhtma</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1efhnex</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's time I stopped lurking... </t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efhnex</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1efhigp</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Got my first PPU order!</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efhigp</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1efhd2f</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I would never have known about these neons if it wasnt for Color Clubs Mystery Sale 😳</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efhd2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1efhcnv</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Nail Polish Collection</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efhcnv/nail_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1efh3x0</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is this? I think it fell out of the packaging of some nail stuff I had ordered for my daughter. </t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpfwlj688kfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1efh0nt</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Polished For Days - Barbie on the Boardwalk (PPU Rewind ‘24)💕</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efh0nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1efgidn</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Amazing sparkle from this Beetles set!!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efgidn</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1efghzp</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about new EDM color (PR photos) </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efghzp/question_about_new_edm_color_pr_photos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1efg1ox</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Mooncat Acidic (mmmm 🧀 Mani)</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efg1ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1efg1hu</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Sassy Cats Sugar Coat Everything</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efg1hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1effds1</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>diy flower bb</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1107cnuttjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1efexqj</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mood ring - cirque </t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efexqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1efemca</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Green glitter jelly ombre 🥝🧚✨</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ptzv4k0onjfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1efekne</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>I never thought she’d be mine 😭</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxoihtocnjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1efei7w</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efei7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1efeflz</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Vetro Sparkly 90s vibes</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y481rjd7mjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1efe6bi</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Lounging in bed w/my cat when I looked over and was blinded by the glow 😎</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efe6bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1efe1ij</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>mooncat stolen ambrosia</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efe1ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1efdw2g</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Anyone Ever Use Cuticula's Base?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efdw2g/anyone_ever_use_cuticulas_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1efdhg4</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Went to the dollar store 😂!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efdhg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1efdbna</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Jen &amp; Berries - Depth Perfection</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efdbna</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1efd8md</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>*scrunched face* not sure if I like it on me. Opinions please</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efd8md</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1efcevt</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I Axolotl Questions</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2bmfvqkt6jfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1efbu8x</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>She's giving amber, she's giving marigold, she's giving honey 💛🐝</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efbu8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1efbe43</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>First ever PPU order!!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efbe43</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1efb9x4</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>PSA esp for olives: Mooncat Ghosts of Hecate has a yellow base</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efb9x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1efb1dn</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to start a collection of a quality brand gel polish. Suggestions?  </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efb1dn/i_want_to_start_a_collection_of_a_quality_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1efarp4</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>🖤❤️Deadpool &amp; Wolverine💙💛</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efarp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1efai91</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>What do you do with polishes you don’t like/want anymore?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efai91/what_do_you_do_with_polishes_you_dont_likewant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ef9jsn</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>What Are some good pearl/chrome powder Brands?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ef9jsn/what_are_some_good_pearlchrome_powder_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ef99yg</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>3-D nail art with Seche Vite top coat!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef99yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ef93w5</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Any recommendations for re-bottling Mooncat?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ef93w5/any_recommendations_for_rebottling_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ef90rf</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Which nail shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef90rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ef7uyv</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>I am just obsessed with this combo. Cirque Mermaid Grotto + Phoenix Ice Delight</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a08dage2aifd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ef7szs</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello Reddit Laqueristas! I DESPERATELY NEED YOUR HELP! </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7szs</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ef7p4y</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Holo Taco’s Mixed Emotions Collection - Review (3 slides)</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7p4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ef7nxf</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>How to achieve nail goals</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7nxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ef7a86</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Favourite drugstore shades?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yodvqdi6ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ef6rup</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Color and undertones of nailpolish, lipstick and outfit have to match perfectly.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j2htd2u2ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ef6q5h</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>BKL Choose Life</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hvsv2zgh2ifd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ef6gwy</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>What are your holy grail products for your hands?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dvwsqjo0ifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ef698c</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time using the sponged on flakie technique </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef698c</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ef5ds3</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Studio Ghibli themed nails</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef5ds3</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ef55px</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>This weeks mani!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daomxflgrhfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ef40mt</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does my middle finger nail look like this? </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef40mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ef3oeb</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>ILNP - Carved</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dtv699tghfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ef3hm0</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>For those that use IKEA storage drawers for your polish, do you prefer the Helmer or Alex drawers?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ef3hm0/for_those_that_use_ikea_storage_drawers_for_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ef3el3</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Jelly disappointment </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef3el3</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1ef2tzp</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>guy here who wants to experiment more with my gender expression - i don't have nail polish so i painted these with acrylic paint !! :3</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg9p8vjpahfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1ef2kvn</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Vamp collection launching soon.</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef29n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1ef267g</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Surprise Crelly!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef267g</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1ef1yk9</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Limited Edition Dior 796 Dupe</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuf6ggyh4hfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1ef0rw0</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I'm looking for alternatives to Bell-Bottom Blues</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef0rw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ef023k</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Arcana “My Life as a Shrimp”</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef023k</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1eezsex</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Life as a Shrimp 🦐 </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eezsex</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1eezkwt</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>my husband's favorite nails</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eezkwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1eezj19</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>What is the chrome-iest, most mirror-like metallic nail polish?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eezj19/what_is_the_chromeiest_most_mirrorlike_metallic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1eez1kn</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>This colour is called siren🧜‍♀️🤩</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o7bcondigfd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1eeyp76</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>How on earth do you get pale sheer colours non-streaky?</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/KWLFxFj</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1eel631</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>The best base coat?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eel631/the_best_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1eeo44w</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Mint Skittle</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fztio4eu8dfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1eexpfd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>July round up</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eexpfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1eevpha</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eevpha/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1eeulvy</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Shortie manis in July</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eeulvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1efnaax</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Does anyone know how to achieve this type of gemstone effect?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qoz96ctylfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1efn208</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>advice on where to get stuff pls</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1efn208/advice_on_where_to_get_stuff_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1efml7b</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>How can I improve on character art? (Anime specifically)</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efml7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1efm4rv</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best nails evah.. </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efm4rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1efj866</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NYC nails for my trip soon </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efj866</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1eficxw</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>ruffle my melody 🤍🎀</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eficxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1efhcpf</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>My first set of DIY press ons!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouslu5fcakfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1efer37</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>nails I did in this beautiful color 💙</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4qgksurojfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1efeemj</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Nail Art Tutorials</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://youtube.com/watch?v=KIL-5gG_FT8&amp;si=oU_yiKneZlXZ-iDw</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1efe6pj</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Nails i made</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwyfh3p8kjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1efe4ic</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Nails💙💙🩵i made</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hjey6trjjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1efdva5</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm already practicing for Halloween! 🎃 </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6im92nlthjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1efdmtq</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Done by myself </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bklfzmd0gjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1efdlpa</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxm3getrfjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1efdl36</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi from Canada </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smx4j90nfjfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1efcxq8</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>First time trying anything other than a solid polish. Can’t wait to do this again!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efcxq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1efahyf</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Most recent nail set </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7r04jb8tifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ef9vae</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Milky silver nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef9vae</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ef9h25</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Neon Lights Nails</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4n4j5u3mifd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ef8f5x</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat turning yellow </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ef8f5x/top_coat_turning_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ef7skp</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Soo in love with flowers and 3Ds right now :))</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef7skp</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ef6w89</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>regular nail polish on natural nails</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef6w89</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ef6got</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>MANicure!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef6got</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ef5llk</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Olympics Nails!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ffasjluhfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ef4sag</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Moon nails</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef4sag</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ef1bwh</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My Nails</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l43hkgnyzgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ef0m36</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Anyone else here a fan of Harry Styles? 🍉🥝</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaji27qmugfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1eezw9p</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Pinks and dots 💕</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlvfnx29pgfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1eexlkg</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So cute ☺️ </t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7bufpuco5gfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1eexc9o</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>My first ever set of gel polish nails.</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw4bpij53gfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 31 08:09:12 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C501"/>
+  <dimension ref="A1:C674"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8950,6 +8950,2947 @@
         </is>
       </c>
     </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1eggw7v</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>First time with glue on extensions</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2oyu4sl01tfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1egfd0m</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail tech did a fantastic job </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf021wh9jsfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1egf5jh</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I've chewed my nails to stubs my whole life and this is the first time i feel they look pretty</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a8khmmxgsfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1egf59r</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Summer themed nails! 🏝️</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egf59r</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1ege87d</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>A little extravagant but I love them</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u142zr657sfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1eget92</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">does anybody know why my uv base coat is slimy? it’s brand new 😭 i’ve used this brand many times before. </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/46bid3g9dsfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1egei8q</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Anyone able to identify these three colors?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lcvsn9y9sfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ege4hp</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Does the color suit my skin tone?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/retvype36sfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1egdrzj</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Broken nail bed</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ulk3vjp2sfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1egd1dq</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Gel X length</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egd1dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1egcsdd</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>An update for the red rocket/condom nails 😅</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4jdto9btrfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1egcje6</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Is there such a thing as gel ridge-filling base coat?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egcje6/is_there_such_a_thing_as_gel_ridgefilling_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1egchrd</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Did I get a bad set?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egchrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1egaz6y</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>My art vs inspo pic! Inspo from @Noellefuyunails on IG</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egaz6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1egce84</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Coordination moment with my bf 💖</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uj0tuftprfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1egc69e</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Neon Dots</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egc69e</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1egburn</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Went bright for once! Kinda fun and funky 🌼✨</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egburn</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1egbdnn</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Did my nana's nails for her vacation!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2faaht1xgrfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1egaoxs</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Most recent nail art vs. my first attempt at nail art </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egaoxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1egai2g</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Can you pre paint and design Gel X nails  before applying or do they need to be clear when you do?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egai2g/can_you_pre_paint_and_design_gel_x_nails_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1egafx6</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Structured mani vs hard gel</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egafx6/structured_mani_vs_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1eg9nk8</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Blooming gel round 2!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg9nk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1eg92wu</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>A Saturday at the Farmers Market</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg92wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1eg80gw</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Natural nails gel manicure</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg80gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1eg8hii</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about acrylic &amp; polygel: how do I prevent flooding the cuticle?? I’ve tried so many times and I need advice!! </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg8hii/question_about_acrylic_polygel_how_do_i_prevent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1eg8u3p</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>My quickest set yet!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mazamvxsvqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1eg8wbr</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>First time making press ons</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh74h978wqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1eg8r4i</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun little yellow purple checkered moment </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vyknxc4vqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1eg7y2v</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Chrome with LE’s High Shine Soak-Off Top Coat?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg7y2v/chrome_with_les_high_shine_soakoff_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1eg81xr</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>With high nail salon prices what is appropriate for tipping?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg81xr/with_high_nail_salon_prices_what_is_appropriate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1eg7dw0</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>I accidentally cut my nails too short but I still want to do them with Gel X - Is it too risky?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2q5rhqzgkqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1eg6yat</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>How do I clean polygel off my brushes?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg6yat/how_do_i_clean_polygel_off_my_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1eg6zve</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time doing polygel </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg6zve</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1eg6zpa</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>What is the most protective shape for growth?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg6zpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1eg6y3u</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🫐 🩵 💙 blueberries. </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg6y3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1eg6evz</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg6evz/birthday_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1eg6e83</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>100% natural, this is wild!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4320r8xcqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1eg64ja</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Paw print nail with acrylic cat pinky</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tk5hce3waqfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1eg5x3i</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>what are we thinking😏</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg5x3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1eg5kpk</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Nail hardener?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg5kpk/nail_hardener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1eg5gqy</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>boyfriend's manicure from today</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71kpbdq36qfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1eg5cga</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>loving these so much</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8x0ue795qfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1eg5brm</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Last set before culinary school</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8eheef45qfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1eg4ny5</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Y2K</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg4ny5</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1eg4oge</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>What type of acrylic nail does Glamnetic use?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg4oge/what_type_of_acrylic_nail_does_glamnetic_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1eg4s95</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Appreciation post</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg4s95</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1eg4g8v</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Cottagecore Girly for Life</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qno1xmbtypfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1eg4dmi</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>🐟 Painted Polish Slammin' Salmon on my fingers and Wish Upon a Starfish on my toes. 🌊. This color combo is giving Golden Girls couch vibes and I'm here for it. 🤩</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg4dmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1eg439x</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Pink Pony Club nails by @paonails_spa 💅🏻</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82kte6mawpfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1eg3x8e</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Help me</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg3x8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1eg3kni</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time ever!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg3kni</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1eg3vhg</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Before/after pics are just so satisfying 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg3vhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1eg39wa</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Nails done for Miami ✅</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnljb6khqpfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1eg36aa</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Press on haul</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rkegorvpppfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1efzita</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>any nail care tips?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofpglv4pzofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1eg0slf</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Do any of you have eczema and use cuticle remover?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzp27epw8pfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1eg2b8u</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>any tips to improve my nail art?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1t8k9aojpfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1eg2b4y</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>When your nails match your gaming setup</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg2b4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1eg29bs</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>first time getting aura nails and gems! what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcwecjlbjpfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1eg1vbw</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Secret to growing your nails hard?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eg1vbw/secret_to_growing_your_nails_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1eg1ace</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>This weeks nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg1ace</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1eg11fb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>red cherry set done by me</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg11fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1eg09gd</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My niece used me for practice :)</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg09gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1efzi24</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>What’s the verdict? Too bulky?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efzi24</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1efz5jq</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>inspo pic help?! inspo pic found on trendynails.com</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whz51uq5xofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1efww9c</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Why does my builder gel go soft and tacky after about a week?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efww9c/why_does_my_builder_gel_go_soft_and_tacky_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1efyvp7</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Can someone explain what im doing wrong that my polish looks like this</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d42at7l6vofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1efz337</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Olympic Gymnasts &amp; their nails</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efz337/olympic_gymnasts_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1efyvav</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Gloss vs Matte - thickness?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ogq4wq3vofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1efykjb</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>It's like I'm walking around with Arizona Tea! I'm in love!</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efykjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1efy6a4</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Custom-fit at home nail recommendations?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efy6a4/customfit_at_home_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1efy1qb</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>I am a guy and I painted my nails by myself for the first time, I would like to improve tho :)</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efy1qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1efxwep</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I recreate this type of nail and how can put on the stickers at home? </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x15pszi6oofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1efx58d</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Kicks n Nails👟💅</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9767wmsoiofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1efwrvg</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Kitty claws</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efwrvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1efwmw5</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>I like these V-shaped French ones more, what do you think?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjdq2uz6fofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1efwmrk</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Fancy Roses 🌹✨</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efwmrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1efwk85</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Best places to buy press on nails</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efwk85/best_places_to_buy_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1efwbhn</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Had my nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0txq7wxcofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1eftocq</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Oh how far I’ve come in my nail journey 🥹</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eftocq</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1efvs3i</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to have balance of beautifully nail colors and healthy nails? </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efvs3i/is_it_possible_to_have_balance_of_beautifully/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1efw30w</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Some of my recent nail art 🥳</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efw30w</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1efvuks</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>4 months on prenatal vitamins</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7cb87wl9ofd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1efvjz5</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Mermaid nails look amazing on me 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9owprjk7ofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1efvhmm</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>My nail girl really outdid herself</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obqm1ns27ofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1efoffr</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Top Coat Recommendations</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efoffr/top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1efqa0d</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>What should I learn first?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efqa0d/what_should_i_learn_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1efuuu6</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Mermaid vibes for holiday 🦪</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efuuu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1eftr9u</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Nail ideas for short nails</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvmq4kngunfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1eft3f1</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>My nail tech did an amazing acrylic nail set for my birthday week :)</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eft3f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1efqv56</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails done!! let me know if u like it </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh2fy0345nfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1efqtq7</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Blue and Yellow Combo</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn0hkinp4nfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1efqir8</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Mermaid wishes</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60uz6skn1nfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1efqekm</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking good in my mermaid NailArt </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5gaczvi0nfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1efpw2p</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Various home jobs this year 💐</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efpw2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1efpaz5</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Had a go at painting my first ever character nail. Ponyo 🐟❤️</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efpaz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1efoulf</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Gel polishes</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efoulf/gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1efolvu</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>UV nail polish still a thing?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1efolvu/uv_nail_polish_still_a_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1efokmq</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>New set of very long chrome acrylics, how do they look?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyd941j5fmfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1efohsl</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>I am old nail eater, what to do to cure this appearance?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly5nza84emfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1eggqa9</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>First ever attempt at nail art! First one with my dominant hand, the other was an attempt with my non-dominant hand haha!</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eggqa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1egbktc</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Sally Hansen Hard as Nails: Made in Jade</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40sjuxknirfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1egfmhs</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Glowing soft blue combo</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tpm8p59msfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1egejyf</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>30c Luodanqi blue</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/G9cblbY</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ege3wq</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>1st attempt at french tips</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8xsr52t5sfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1egcpkl</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>ILNP ELECTRIC SUMMER compared with Flower Child, Fairdust and Bluebell</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egcpkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1egch15</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Polished For Days - Fluorescent💡🩷🧡</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egch15</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1egcgnh</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Mooncat dupe help? ❤️</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gln05e5eqrfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1egatuk</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Mysterious Uranus ✨</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9irjvom5crfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1egar5h</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super happy with Eternal Nail Enamel Polish! Definitely worth a try if you’re looking for polish with limited ingredients that dries evenly! </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egar5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1egajg8</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco is my favorite! </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1n4m7sp9rfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1egaciq</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Getting back into painting my nails and first time trying ILNP after seeing posts here!</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egaciq</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1eg9ujs</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Jelly gel x</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg9ujs</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1eg7pay</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Nail of the week</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46scc5pumqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1eg90gt</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>A fun lil summer combo</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gc42e56xqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1eg8t8o</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Feels like I have jewel beetles on my nails!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg8t8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1eg8mf4</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>{PR} Glowstick by ILNP</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsi429u1uqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1eg8ksx</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Dumb question is the Sun UV LED lamp a UV lamp or an LED lamp or I guess both?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg8ksx/dumb_question_is_the_sun_uv_led_lamp_a_uv_lamp_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1eg8j02</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>What’s the manicure LPT that improved your nail game the most??</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg8j02/whats_the_manicure_lpt_that_improved_your_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1eg8a8e</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>First LynnB order.. did I go overboard? 😅</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg8a8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1eg88k0</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">May I have some polish recommendations? </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg88k0/may_i_have_some_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1eg85fr</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Vampire Nails</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcmxwbzcqqfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1eg7hrm</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Blossom’s Firebreath, Don’t Cry Bubbles, Fool’s Gold and Speed Demon</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg7f13</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1eg7e2j</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>If I’m finishing my manicure with a QDTC, do I have to wait for each step of polish (base coat, 2 layers of coloured polish) to dry before finishing up with a QDTP?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg7e2j/if_im_finishing_my_manicure_with_a_qdtc_do_i_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1eg6aq1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>What Addiction? - The Abyss</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg6aq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1eg619y</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Thermals, but reverse it</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/kdiABE6</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1eg60zd</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Opinions on scented cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg60zd/opinions_on_scented_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1eg5xfs</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>💚Shift in Perspective 💙</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg5xfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1eg5f15</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Horseshoe Magnet</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg5f15/horseshoe_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1eg4y4q</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer - Macaw Me Maybe</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yevcithc2qfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1eg4nq3</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Sugar, Spice, and Everything Nice</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/RcjDzoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1eg4929</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>summer time, pool vibes!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg4929</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1eg48fh</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Mooncat “Merkitten” and Holo Taco “Deeply Superficial” on accent nails</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg48fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1eg3z2l</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Why is my polish taking so long to dry?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg3z2l/why_is_my_polish_taking_so_long_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1eg3w1e</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Late to the horseshoe magnet party…</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q9bw2snuupfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1eg2ad5</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>My Top Coat made my manicure soft?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eg2ad5/my_top_coat_made_my_manicure_soft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1eg0x9c</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Jior The Tea on the Manatee</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3yrzl03t9pfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1eg09zz</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Pretty enough to paint on a ham</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg09zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1efzs86</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Frog Nails 🐸</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efzs86</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1efzntu</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Good base and top coat for working hands?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efzntu/good_base_and_top_coat_for_working_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1efzkfu</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Some sunshine for the feed 🌼🌞</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efzkfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1efsjo1</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>This Formula 🤌🏼 Windows Down, Radio Up</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efsjo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1efywp6</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Beaux Reves</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efywp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1efwbk6</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Product suggestions for a newbie?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1efwbk6/product_suggestions_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1efxz5y</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Omg Chicago Fire! 😍</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efxz5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1efx0bd</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Multicolor ferns!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efx0bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1efwgao</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Cirque Colors solid color comparison from my last haul</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ef6fph</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1efwdra</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>ILNP Masquerade (H) + Starrily Nova Beam , 🧲 on ring finger. Ft. Butterfly pea milk tea with two shots or espresso and milk foam on top. Delicious</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e6ktz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1efw10w</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Derpy lil Penguins</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k32ssw9vaofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1efu16i</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Clionadh Salt Watermelon Taffy 🍉💚🩷</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efu16i</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1eft4ih</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Looking for a gel polish the same color as Lights Lacquer Clueless! A sheer pink with a jelly finish.</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8pmx33gpnfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1efsu6t</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Everyone needs a bit of sparkle ✨ </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efsu6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1efsjma</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I love shorties!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efsjma</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1efs8jb</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Tried something more subtle</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efs8jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1eggf3r</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>My first nailz</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af7yvfodvsfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1egeoqa</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Nails i made 2022🤎</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srso6c4vbsfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1egejs7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>strawberry nails!!:D</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md8y1kjeasfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ege9hz</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Studio ghibli nails </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ege9hz</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1egauzr</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another set completed </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi6bjrzfcrfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1eg949s</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>A Saturday at the Farmers Market</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg949s</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1eg7gyr</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Aspiring Nail Tech in Toronto</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg7gyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1eg7625</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>some nails i’ve done! which one is your favorite? 🥰</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eg7625</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1eg6z5m</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Could you give me your oppinion plis 🥹 </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sn605nz9hqfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1eg655z</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Paw print with acrylic cat pinky nail</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13nnqo11bqfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1eg3u4c</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>It’s like a fairy garden 😍</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqwyxqrhupfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1eg1bag</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Fairycore style🧚🏻‍♀️ featuring my antique ring.</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3c640dncpfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1efzyde</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Pixar nails</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efzyde</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1efzjuq</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Matched my nails to my ring</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8k1xfjwzofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1efx45l</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Dried flowers encapsulated in builder gel</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dn5zgmliofd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1efwphm</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Fancy Roses 🌹✨</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efwphm</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1efw8h2</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>my first two tries doing nail art! 💕</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1efw8h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1efqi1i</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Mermaid wishes</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxxpuc3g1nfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1efomlu</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>UV nail polish still a thing?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1efomlu/uv_nail_polish_still_a_thing/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug  1 08:09:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C674"/>
+  <dimension ref="A1:C843"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11891,6 +11891,2879 @@
         </is>
       </c>
     </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ehb7c4</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Baby boomer nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehb7c4/baby_boomer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ehat5j</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Nails made by me 🥰 i was aiming for mermaid vibes and ngl this is my proudest set.</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehat5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ehamxr</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Maid of honor nails 🤍✨</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehamxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ehaibj</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">July Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j043aii670gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ehabbk</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>I think she likes them 💕</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehabbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ehaanc</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My espresso shot mirror is to look at my nails lol </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehaanc</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1eh9tpo</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Infilling clear BIAB help</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh9tpo/infilling_clear_biab_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1eh9yg8</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Green Glass Leaf Nails From a Recycled Bottle.</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh9yg8/green_glass_leaf_nails_from_a_recycled_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1eh9iot</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Help! I need some inspiration I have a nail appointment Friday morning! Please post pics!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh9iot/help_i_need_some_inspiration_i_have_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1eh9i09</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>My newest set</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oomc4y24vzfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1eh9dlr</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Manicure love</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh9dlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1eh90v9</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few of my favourite designs from this year (so far!) </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh90v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1eh8dk3</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>DIY Acrylic from Amazon- waste of money/dangerous?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hppk7tjaizfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1eh89fs</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>It’s the press ons girl again</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpnxvky0hzfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1eh849m</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these good? </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh849m</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1eh82fn</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>First time getting nails done! Gel x ones!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh82fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1eh7inj</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>nails are suddenly more flexible even with nail polish on</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh7inj/nails_are_suddenly_more_flexible_even_with_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1eh7v2z</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My pretty summer nails! (Cursed nail photos included) </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh7v2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1eh7i04</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>The more I look at them the more I hate them 😭</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh7i04</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1eh7d02</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How long does Jello-Jello Peely Base last on you? </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh7d02/how_long_does_jellojello_peely_base_last_on_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1eh719f</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>First time doing poly gel, how did I do?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jk8wpjz4zfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1eh6qbt</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Should I pant over this? I wanted light pink but this is giving raw chicken</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my4k1rz02zfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1eh6pd7</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for the first time since becoming a mom </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/octgey3r1zfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1eh5dip</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Started nail art again</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzsak8nkpyfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1eh61g7</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Too soon??</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt4epihjvyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1eh5st1</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Hey guys, I’m struggling to decide which colour I should do on my nails to go with this outfit for a wedding event - what would you recommend?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76lce3wdtyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1eh5rgr</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>When is it too late to get your acrylics filled?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh5rgr/when_is_it_too_late_to_get_your_acrylics_filled/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1eh567v</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>questions about sns nails</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh567v/questions_about_sns_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1eh55j3</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Grievously Cut My Finger While Cooking Lunch…Made Sure the ER Doc Left My Nail Exposed for My Afternoon Manicure</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh55j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1eh54ji</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwi8bw3hnyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1eh4w6h</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>fwoggy,,, 🐸</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqc0mltflyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1eh4w3p</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Airbrush look without an airbrush machine :)</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh4w3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1eh4r4d</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Best non/low tox gel like option?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh4r4d/best_nonlow_tox_gel_like_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1eh4ljn</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte nails </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yw8ua2uiyfd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1eh2thj</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Is it possible to use chrome with tacky gel top coats by wiping inhibition layer?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh2thj/is_it_possible_to_use_chrome_with_tacky_gel_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1eh2v45</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Rubber Bases for Darker Skin</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh2v45/rubber_bases_for_darker_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1eh2v0g</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal 1.5 weeks growth, I’m spending so much having to get them done every week </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh2v0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1eh2q7b</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow Cateye 🌈 </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y0vcfqlu2yfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1eh1l13</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dhewzdftxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1eh2dow</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Blush nail method?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh2dow</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1eh26zc</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Very first attempt at Gel-X nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh26zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1eh1ogt</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>GELX I did on a client 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6eqpbeu7uxfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1eh1dzp</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh1dzp/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1eh16my</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would you have these redone? </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbiaaknaqxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1eh0z2q</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>They used to be called empress tips but then rebranded and I cant remember the name!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eh0z2q/they_used_to_be_called_empress_tips_but_then/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1eh0ywy</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>New set of Claws</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh0ywy</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1eh0yww</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Punk rock, but girly 🖤</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwysaq2moxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1eh0skx</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Love me some chrome!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pbvuoduanxfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1eh0qka</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Festival ready 💅</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh0qka</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1eh0phq</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of my animal print nails? </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i87s7h7nmxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1egzsm6</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Thoughts on this French tip manicure? First time getting French and dip, not sure if i like them!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8icq1hcsfxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1egzp25</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Ruby for my fellow July birthday buddies</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egzp25</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1egzj6n</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>i missed my claws</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egzj6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1egzbxi</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Is this website legit? kodiprofessional.com</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egzbxi/is_this_website_legit_kodiprofessionalcom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1egzalb</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First nails ever! </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74pfzks5cxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1egz69t</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>foils didn’t transfer perfectly but that’s ok 👼🏻</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egz69t</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1egxmjt</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second attempt at nail extensions </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3smtvv20xfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1egynob</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Ombré nails for the first time 💅🏾</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egynob</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1egyhho</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>first time doing gel x</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egyhho</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1egybcb</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w64kk6ru4xfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1egyanb</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>getting better with acrylic but looking for tips</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egyanb</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1egxw8f</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>When your nails match your soap bottle…</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egxw8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1egxu60</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I did today! </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egxu60</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1egx6mb</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Coworker told me these looked cheap ?!?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb0v984uwwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1egurfp</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting my nails done for first time </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egurfp/getting_my_nails_done_for_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1egwfx5</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>obsessed w my magnetic gel nails from korea 🥹</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egwfx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1egw96r</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Really loving my nails today!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5al2pne2qwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1egvs6k</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set of press ons </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvy2h93nmwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1egvhel</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>First time doing a design!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egvhel</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1egvnq5</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>press ones!!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egvnq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1egv70e</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Wedding nails!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc0pf2fhiwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1egv1b3</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>First time trying the popular 3D hard gel trend</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egv1b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1egumkw</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mine 😍 10 min getti g ready for wrk mani #frosted </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fv1y5euaewfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1egsn2c</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Glow Nails progression :)</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egsn2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1egsm5c</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>I need help guys! I have a nail appointment on Friday please send inspo! This is my current set</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp9qih020wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1egthil</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Help! How do I minimize the gold without getting another manicure?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfhfucxa6wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1egu0yg</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>First time removing my cuticle (Russian manicure style). Did I do a good job? Any advice?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egu0yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1egtzfm</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with teal today </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzmj1hhr9wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1egtx09</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at gel tips </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bd409bc9wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1egtq72</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Kp60 manipro drill</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egtq72/kp60_manipro_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1egtllw</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Summer set</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40thvjo37wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1egtb8x</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Would you pay 145$ for this before tip?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z6582925wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1egtb79</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies for day 2 of the Bar Exam 👻</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vjx80225wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1egt9jy</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Dreamy Set</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egt9jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1egsy5p</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple colors &amp; a holo taco </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4xw6v1f2wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1egs7dn</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Neutral nail shape? What shape compliments my hands?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egs7dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1egs65c</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite set ive done on myself... I LOVE them! </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egs65c</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1egryo4</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Chrome powder and gel polish 💗</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egryo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1egp08r</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Any tips so gel polish doesn’t mess up my nails?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1egp08r/any_tips_so_gel_polish_doesnt_mess_up_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1egnxj0</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>3d flower trend set</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egnxj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1egksuy</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Can I get acrylics on what’s left of my nails?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dipogqv0bufd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1egrnaf</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>gold french</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro64ukd3tvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1egrmfu</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trying to grow and shape my nails </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1woj7stwsvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1egqstf</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Can I polish over this until it grows out?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6mark01nvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1egqbgc</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairy garden </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2qjkwnijvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1egpp6a</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Christmas in July</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egpp6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1egpjfk</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and pearly </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egpjfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1egpd6r</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>2 weeks ago I started doing nail art on my natural nails. I this this is my best work yet!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05bit7pocvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1egopsi</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Rainbow set 🌈🌸</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/701cnw6v7vfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1egochu</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Hyper-Realistic Nail Trend</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pt8bari25vfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1eha2si</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Allergy risk with custom press ons?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eha2si/allergy_risk_with_custom_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1eh904g</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>It's my baby's birthday so I painted my nails with ILNP Birthday Suit</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh904g</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1eh7j41</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Looking for minimalist/clear nail polish suggestions</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh7j41</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1eh5v1p</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>where my people at?? brown and wine jelly things</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eh5v1p/where_my_people_at_brown_and_wine_jelly_things/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1eh5t4a</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Psyche Minerals’ Ghastly Smell is so sparkly! ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh5t4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1eh5cn2</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Seeking Opaque Baby Pink Lacquer</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny4sx2adpyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1eh4mfg</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Haunting Your Own House</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dstx7pz1jyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1eh47si</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Finally successfully water marbled!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh47si</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1eh42b6</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I WAS ABSOLUTELY FLOORED</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh42b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1eh3ngi</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>If both of these Futuristic nail painting tools existed which would you prefer?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh3ngi</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1eh3ily</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Be Mine ❤️</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/xxZCfsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1eh3ce5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>The Natural Order - Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9u1dhfa38yfd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1eh34vj</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deco Beauty's Gorgeous Bottles </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh34vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1eh32cg</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - The Diabolical Mojo Jojo!! Luckily no issues with my bottles </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh32cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1eh1prk</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>When the combo looked cuter in your head…</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh1prk</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1eh1kid</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Just tried magnetics for the first time and Deep Space is ridiculous 😍🥰</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh1kid</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1eh19s3</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For those of you who use Helmers for your collection, how much weight does each drawer hold? </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eh19s3/for_those_of_you_who_use_helmers_for_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1eh15ae</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Hot damn.</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh15ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1eh12ok</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">perfume removing polish </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eh12ok/perfume_removing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1eh0x7p</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Nail pics in the car</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnyd9d99oxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1eh0sbz</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>I blame y’all for my first Lyn B Designs order 💅</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzwjjf39nxfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1egzs5k</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell + Growing out my nails!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egzs5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1egzks2</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Sassy Sauce “High Jinx”</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egzks2</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1egylld</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Mooncat Pixiestick vs Death Valley Abalone?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egylld/mooncat_pixiestick_vs_death_valley_abalone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1egyhn1</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Mooncat Neverland with Roses</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to5rq8286xfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1egxube</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>help strengthening nails??</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egxube/help_strengthening_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1egxje1</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Polished For  Days - Goblins and Ghoulies!!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p3z360gzwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1egxbgu</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>PPU Rewind- Lümen Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egxbgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1egwqd8</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Summer Blue 🌊</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egwqd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1egwfnz</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">okay lovelies, can you share the like to the magnet that makes you create the velvet look? and share some tips?? </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egwfnz/okay_lovelies_can_you_share_the_like_to_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1egwe4l</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Whatcha Magnetic 🧲⚡</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egwe4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1egw7i8</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Express Yourself</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egw7i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1egvj1m</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Nails Are Engagement Photo Ready! 💍</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpxu16jakwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1egvbbi</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>How would you jazz up this creme?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o16j6lxcjwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1egup2y</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nail hardener issues. (Sally Hansen) Bunk product or bad use?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egup2y/nail_hardener_issues_sally_hansen_bunk_product_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1egrizs</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Peel-off/Soak-off Gel Nail Polish for Press-ons?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egrizs/peeloffsoakoff_gel_nail_polish_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1egs21y</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Mooncat Whiskey Sunrise dupes</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egs21y/mooncat_whiskey_sunrise_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1egqi15</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Mooncat</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egqi15/mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1egtkx1</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Holo Taco Rage Bait</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/autq3n4z6wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1egtaks</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies for day 2 of the Bar Exam 👻</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj712jdx4wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1egt6g6</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Blueberry mani and muffins 🫐</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yep51pn34wfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1egsj8t</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>BKL Elden Beast</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egsj8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1egr988</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Barbie meets magical girl</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egr988</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1egqvpi</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>No one told me PFD’s Baja Blasted GLOWS under black light!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egqvpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1egokr1</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Cirque Colors Dove Jelly 🩶</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egokr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1ego38v</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Poison - velvet</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ego38v</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1egmcv1</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Your favourite base and top coat for a very LONG lasting manicure? No chipping + TIPS &amp; TRICKS?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egmcv1/your_favourite_base_and_top_coat_for_a_very_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1egkqy4</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Healthiest Base Coats?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1egkqy4/healthiest_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1egk6tb</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Is it ✨giving✨ or….</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2ikxqjq4ufd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1eghu1b</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Best nail glue for sensitive skin?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eghu1b/best_nail_glue_for_sensitive_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1ehao5w</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>🦋butterflies and cherries🍒</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oye87zh690gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1ehan3n</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Nail oils and strengtheners</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ehan3n/nail_oils_and_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1eh91p3</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Mermaid nails attempt</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh91p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1eh7nkc</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Rojo baby stilletos</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh7nkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1eh6nhj</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>i love this nails 🖤😮‍💨</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh6nhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1eh56zq</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>My take on Bridgerton nails!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eh56zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1eh4t3i</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Combines with my case</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19ycfacnkyfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1egxuvl</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I did today! </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egxuvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1egvfjv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Goth mermaid press ons</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ejf9xn4kwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1eguqps</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My work </t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cdc7556fwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1eguctz</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>what do you think of these nails I made?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k820tp2fcwfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1egt4nt</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Butterfly Nails!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egt4nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1egsihm</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>How long does it take for gel polish to dry?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1egsihm/how_long_does_it_take_for_gel_polish_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1egqck3</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Koi fish!!! </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bgmxeorjvfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1egpngg</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>any help?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19y4oi6qevfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1egny7v</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried foil for the first time </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3wjnca22vfd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1egnutu</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>3d flower trend set</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egnutu</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1egnkam</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1egnkam</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1egkf04</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the right combination of colors, for cherry lovers </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pf761wt6ufd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug  2 08:09:19 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C843"/>
+  <dimension ref="A1:C1015"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14764,6 +14764,2930 @@
         </is>
       </c>
     </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1ei3ydz</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple but pretty </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jii42tfdd7gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1ei27ib</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Nail salon advice</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ei27ib/nail_salon_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1ei25q3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>growing nails out</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ei25q3/growing_nails_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1ei1hqx</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie Pink </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sawhy9y7l6gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ei0uzx</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm a nurse with tiny hands and short nail beds, so I don't have much real estate to work with. But I'm loving this new set I did on myself recently :) my nails are short, life's short, have fun, taste the mermaid rainbow 🌈 </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei0uzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ehwu4k</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Natural nail problem</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouqqzuh8e5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ehxn8l</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to do if an acrylic nail gets bumped and rips off the nail bed a little? </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehxn8l/what_to_do_if_an_acrylic_nail_gets_bumped_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ehxydu</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>What to ask for? New to nails please help!!!</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehxydu/what_to_ask_for_new_to_nails_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ehyvc1</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail extensions </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehyvc1/nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ehys10</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I do with these nails </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehys10</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1ehzb06</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I got vs what I asked for! Inspo from @monika_nails on IG </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehzb06</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1ehzclz</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Summer Cherry Frenchies</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehzclz</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ehzm4w</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>I think this is my favorite set!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehzm4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ehzofu</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Nail help!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puvl0o0m36gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ehz93a</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Month long grow out, surprised it has lasted this long </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1c1ixyrnz5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ehx41s</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Tips on using press ons with medium/long natural nails?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwcswqllg5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ehyq28</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Love these press ons! (+ a question)</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fzz0fluu5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ehylnt</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>I like having long nails, and this is the best gel polish I've done so far, but it seems difficult for me to get along with them...</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehylnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ehyl2h</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Bought this press-on set down south, I am Obsessed with the lil peaches!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o1ilvblt5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ehygj7</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Koi fish nails, complete with bubbles 🫧 </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehygj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ehyfn3</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Can you rate my new nail tech?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bd9qvtu7s5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1ehxmd3</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Tips on doing non dominant hand??</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehxmd3/tips_on_doing_non_dominant_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ehxgx6</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My press on nails always pop off in cold weather</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehxgx6/my_press_on_nails_always_pop_off_in_cold_weather/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ehx758</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Bridal nails for my SIL</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4gpyn8lbh5gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ehx23r</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I like men to fear me just a bit...</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03cque45g5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ehws7u</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best set yet on my friend </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehws7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ehvnb6</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails are super bendy and weak and cannot keep a manicure on for longer than a week. </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehvnb6/nails_are_super_bendy_and_weak_and_cannot_keep_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ehvfmf</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Should I get gel or acrylics for school?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehvfmf/should_i_get_gel_or_acrylics_for_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ehvefl</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Enjoying my natural nails lately</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dtooqbc25gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ehv8jz</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>i love having long claws, and this baby pink is the dream 🩷</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opz8s75015gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ehupga</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>First time using nail extensions!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehupga</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ehuoko</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>my first time opting for gold chrome instead of my usual silver ✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edpg9r0lw4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1ehud5x</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Love love love. My nail tech 💅🏾💅🏾💅🏾</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21g2wfq2u4gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1ehu71s</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>1st time sponge ombre 🌄</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehu71s</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ehngeh</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>[MO] Feeling like 95$ + tip was too much for this set - am I wrong?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfbng1ete3gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1ehtndg</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Which nail shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcz36g2eo4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1ehtm4d</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Lavender</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehtm4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ehtc8n</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Light blue shorties for baby boy who is arriving any day now!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehtc8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ehou01</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehou01</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ehsucf</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My latest set (my dream nails!) </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzsbm4t6i4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1eht5e1</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Very random gel nails❤️</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ne3yd5fik4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1eht0j0</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these done today. Did they go too far away from the cuticle line? </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0us0tmmij4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ehsi52</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Worth it ?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em6nr2ulf4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ehsaos</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Nails done by me, I wanted a darker design but didn't have time</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waodn592e4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ehs5vb</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Got my nails done for my birthday today 🥰</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dombt83d4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ehrop1</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetle gel </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehrop1/beetle_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ehmb7e</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Alternative  coquette</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zacs4lam63gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ehrgru</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>my first set!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehrgru</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ehrbfu</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>practicing my own acrylic nails, thoughts? 💞</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehrbfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ehqpxb</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love doing my friends nails! </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp1tvx3n24gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ehq3mm</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>I want to get acrylics removed, what would be the next step?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehq3mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ehpyai</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>After press on</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ges6f0m2x3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ehpx4o</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Pink &amp; orange ombre 🩷🧡</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9o6swjvw3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ehpnr4</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Why does my polish never dry properly?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ckfy14yu3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ehlag0</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Why is this chrome powder not working? Am I doing something wrong? :(</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehlag0</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ehppj9</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Some of my favorites from the last few months</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehppj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ehpoh8</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>first time tryin this gradient greyscale french tip</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4164bn3v3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ehpi37</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I get dip nails shortened? </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avq4lgipt3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ehp1w0</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opening a beverage can with long nails. </t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dkmr2gn8q3gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ehp15y</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel nails! </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0opnek26q3gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ehp0s7</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>a lil clown set i did 🤡</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehp0s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ehoqvq</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Birthday Set for my Bestie 🌸</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehoqvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ehoafu</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>oh my gosh !! i soaked off my extensions last night and discovered my nail broke ! 😭do i cover it with something or leave it?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bknj3k3vk3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1eho5ug</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Set for my anniversary today 💗</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eho5ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ehnwlo</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>First time using press ons. Are the ones on my thumb and middle finger too big?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehnwlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ehncr0</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ehncr0/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ehnscs</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Cateye gel polishes are such a game changer. No more going back! 🤭</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orj6o488h3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ehnfyk</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>a collage/ doodle set!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehnfyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ehnmmi</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>new gel glitter</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehnmmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ehnhhn</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Back to simple neutrals — with just a dash of sparkle</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehnhhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ehn7wr</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Nail student's first time doing gel-ex</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dajte946d3gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ehn5w1</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>It’s giving “mermaid secretary”</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha5awmurc3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ehn298</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>floral milk bath 🌸✨</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehn298</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ehmwv2</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part IX</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aofufr3ya3gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ehms3a</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Peachy glazed nails (chrome is my favourite!)</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7d2f2uz93gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ehmd73</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Nude base, gold leaf, airbrush red &amp; black detailing</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iohyj9m073gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ehmamk</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These are by far the best press ons I’ve tried </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehmamk</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ehm12v</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Been a nude long nail girlie for years, thinking about doing them all short and green?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuwhobfm43gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ehlrvt</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Nails help!!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs4q86nt23gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ehldtw</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Loved this set my nail tech did ($90 plus tip)</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehldtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ehkl6p</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>INSPO NEEDED - silver &amp; red</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehkl6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ehkq2e</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shiny/Matte </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwf70zs5v2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ehkol2</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Mermaid nails</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8z0dtwuu2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ehi0ic</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>So in love with this set!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de51np7bb2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ehezrs</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Which nail shape?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehezrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ehcb1t</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>engagement nails 🤍</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xhhyw4gt0gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ehahxq</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>my first acrylic set. how do you prevent lifting of the nail?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehahxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ehk1sy</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Light Rose</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53dc2sceq2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ehjtdu</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>painted em black!!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkqnwkqpo2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ehjrfj</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I love the colors 😍</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqekdhfbo2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ehjk6c</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>got my nails done yesterday :)</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wousnettm2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ehjgxs</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I'm graduating on Saturday so I had to get them done. Rate them out of 10</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehjgxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ehjguy</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Loved this set for Valentine’s Day💌</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4v43tq5m2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ehizku</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Cherry acrylics diy</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1abxj9tmi2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ehiccp</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>What should I do about this until it heals?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/L9Zw5gS.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ehhkxp</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Rainbow nails</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoqd17g082gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ehhbsf</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>the iconic kiss nails but almond !!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehhbsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ehhavj</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Tried a red flame ombre on my nails</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq95nzuw52gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ehh470</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Summer Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eddsjknh42gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ehgtvt</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>should i change my shape?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehgtvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ei3ek9</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Trying to break my gel habit but the smudged nails are killing me</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ei3ek9/trying_to_break_my_gel_habit_but_the_smudged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ei2jtk</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>How to paint small toenails with gel?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei2jtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ei00vk</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Hot weather calls for neons!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q991o3fw66gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ehz187</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>~*♡*~ Can someone dupe this purple beauty? ~*♡*~</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d981qd0ox5gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ehyqya</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>glisten &amp; glow sales</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehyqya/glisten_glow_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ehyhtv</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>ISO neutral toe color that won’t make me look like a corpse</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehyhtv/iso_neutral_toe_color_that_wont_make_me_look_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ehwwoj</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Miss Lisa Frank</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehwwoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ehwqtl</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Is it supposed to arrive half empty? 🥲</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9jy22zgd5gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ehvsdj</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>If you’re ever in Japan, I cannot recommend these cheap-as-chips cuties from Daiso enough 🥰💖🫶</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urj9ve9i55gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ehvox8</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Ugliest combo yet</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehvox8</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ehvaz6</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>LynBDesigns haul</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04hpwavi15gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ehv3l5</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm mesmerized </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ec3af56uz4gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ehuyu8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Name of technique? </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehuyu8/name_of_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ehunwj</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Dark Omens but make it matte</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehunwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ehttsv</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>✨️Holographic Butterflies✨️</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hb8t4wrp4gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ehte5j</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>First nail design in a while ✨💅</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehte5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1eht8gy</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Crabs is Bugs </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eht8gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ehr89f</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Cat approved manicure</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ligtasbb64gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ehqpfm</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>how hard should my soft gel be when its fully cured?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehqpfm/how_hard_should_my_soft_gel_be_when_its_fully/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ehq40e</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>The sun likes to play hide/seek with me</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdrjhhway3gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ehq375</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first ever set of DIY glue on nails! ILNP Flicker </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5oqteh4y3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ehpnxk</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Prism Polish UK - Turn on the Juice</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mmno5tzu3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ehpnmt</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Show me your BRIDAL NAILS!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehpnmt/show_me_your_bridal_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ehpgdi</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Fair Maiden - Remember The Monsters</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehpgdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ehp6om</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Has anyone ever tried straining hex glitters out of their nail polishes??</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehp6om/has_anyone_ever_tried_straining_hex_glitters_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ehoqr7</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pietro Maximoff (MCU) inspired nails </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehoqr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ehnx8s</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yubaba by Ethereal </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehnx8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ehnjwz</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>It giving “mermaid secretary”</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94k2cifjf3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ehmegu</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Losing my Advent Calendar/Collection virginity</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr1ueq9973gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ehmasq</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>First LynB order! Which one first?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehmasq</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ehm45r</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>First PPU order / Sassy Sauce Wet Spot</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehm45r</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ehk01c</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Discontinued: Diorlisse Abricot Smoothing perfecting nail care?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehk01c/discontinued_diorlisse_abricot_smoothing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ehjxkv</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>This one needed both types of light.</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehjxkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ehjiks</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Pink holo skittle 💗💕</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehjiks</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ehj9l2</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Sometimes experimenting pays off</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yyb6ez0nk2gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ehih04</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>BKL Goddess of Rot</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehih04</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ehibyl</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>First time attempting a free-hand French manicure since overcoming nail biting, I'm a fan!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehibyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ehhnln</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 weeks of my wedding mani and I’m so sad to remove it! </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehhnln</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ehglhq</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>1st time ombré - Lessons I learned…</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehglhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ehglc4</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Sippery Suckers!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35jai7jb02gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ehgcep</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Thinner coats are better! I tried 2 “normal” coats on my left hand and 3 thinner ones on my right. What a difference! Feel free to share more bubble-busting tips.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz4z9yiay1gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ehfx7b</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a shimmery brown?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehfx7b/can_anyone_recommend_a_shimmery_brown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ehfpyx</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Placing my first ILNP order: what are your must-haves?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehfpyx/placing_my_first_ilnp_order_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ehf0m0</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>advice for selling press ons?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehf0m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1eheotv</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>A little DIY 80’s tropical vibe to embrace this heatwave!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkqf3pilj1gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ehehad</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Milky and glowing from within!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehehad</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ehd7h1</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Can you fix lumpy gel polish?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehd7h1/can_you_fix_lumpy_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ehcvq5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehcvq5/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ei3thm</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Beautiful baby blue nailz for winter time🩵🩵</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdz8kb1rb7gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ei3sqg</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Glow in the dark nails</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei3sqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ei37k6</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I want to show u my nails! This is my third time getting my nails done and I can't believe how good they turned out! Do u like them?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei37k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ei1mqz</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Pink summer press on nails by me :)</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei1mqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ei17v0</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>An end of summer/back to school set for August!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei17v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ehzn5q</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Took a while but so worth it!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1xsd8m3a36gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ehze5x</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Breakfast at Tiffany’s Set </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehze5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ehvw9n</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice, should I add something to the blue nails or leave as is? </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5xbkxwb65gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ehuky3</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel nails! </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/enkxqvfqv4gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ehuflk</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>...and all it took was 8 hours and a lot of back pain 🤩</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehuflk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ehsuwe</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Finally get to wear the TNG set I made!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tvnmvxkbi4gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ehrzi3</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>New 💅</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nod1iotb4gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ehr487</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>My black and gold evil eye nails</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vivza6wh54gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ehqi0r</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>free design today 🥰</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cg4tdc314gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ehp91s</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t xml:space="preserve">frenchie approved gradient grayscale french tip </t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehp91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ehp1t9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jewel nails! </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hu89e92bq3gd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ehox74</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Pietro maximoff inspired nails (MCU)</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iigurnufp3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1eho3sw</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Slugs</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71rlntdjj3gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ehk3fg</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I have never done this design before, it is beautiful 😍.</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/378715wpq2gd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ehjiet</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Made these last night 💚</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4j3dhbhm2gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1eheqjo</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>I love these nails 😍</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wouip2z1k1gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ehenfp</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Fun 80’s Tropical vibe… not bad for doing it myself!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn5s3gv7j1gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ehc71k</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Tambourine and butterfly, inspired by Minä Perhonen ⚮</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehc71k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ehbfem</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Mediterranean inspires summer nails</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehbfem</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug  3 08:07:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1015"/>
+  <dimension ref="A1:C1185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17688,6 +17688,2896 @@
         </is>
       </c>
     </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1eixpzn</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Did my second set of press on nails</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31ju1fs2megd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1eixnav</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>One month till Spring 🇦🇺 but I’m ready</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wljhahl5legd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1eixgig</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>First Attempt at Press Ons</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqsg6hhwiegd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1eix8ai</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Funky set!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eix8ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1eix7j7</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Builder gel on top of cat eye = shiny glass effect</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eix7j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1eiwgh8</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My nails look good? I have worn them 3 times and they are press ons from Tjmaxx!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v87yjmdc7egd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1eivwiu</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What do we think ♥️♥️</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gkroy011egd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1eiu1at</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>This orange color got messed up in the sun but is back to normal ??</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiu1at</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1eiuy46</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I did hard gel on my nubs and painted them this cool neon coral color 🦩</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiuy46</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1eiuxhv</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Great Vintage Red!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h408kq4nqdgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1eiu7mk</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">strawberry nails for my bestie :) </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiu7mk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1eitqm0</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Trends?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hnkquyyedgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1eisq5k</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>My finger nail fungus/nail lifting journey</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eisq5k/my_finger_nail_fungusnail_lifting_journey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1eisu89</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Glittered my nails</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eisu89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1eirh50</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>What do you think of this design in white with a touch of blue 🤍💙</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ivuuhoducgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1eiqix8</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Flora from winx club inspired nails</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiqix8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1eisgpl</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Does this look like a good beginner lamp?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwzf3w7c3dgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1eisf96</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Helen when I catch you Helen</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eisf96</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1eis42v</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some more $6 press ons. Obsessed with this brand! </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eis42v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1eis0vd</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Can I use regular paint paint on nails</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eis0vd/can_i_use_regular_paint_paint_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1eis0jb</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Can I use regular paint paint on nails</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eis0jb/can_i_use_regular_paint_paint_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1eiryla</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>How are you my friends? What do you think of this blue color?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka1vnn6tycgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1eirrdz</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>RED🍷♥️💋💄🌹</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eirrdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1eirjx6</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Blush velvet nails</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7jpq9q3vcgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1eirhpm</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6oeh6cjucgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1eirhld</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and orange aura gel manicure </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1za4g2iucgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1eiqnmj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Black &amp; Red 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cty1k590ncgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1eiqj1g</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red nails, yes or no? </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o03gjb7wlcgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1einhtw</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>how do i fix this</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1einhtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1eincp1</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you function in long nails </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eincp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1eilth9</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Capy cuteness</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g9ynfdrjbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1eilhz2</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Would it look bad if I used a 3rd color for a fill in of my ombré nails?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyfwe9u7hbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1eiq2r0</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Love a shiny cat eye</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiq2r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1eipo3g</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This month’s cutie set </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr9o4ymhecgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1eipfhe</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Back to natural nails 💅</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfbuggchccgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1eip4gc</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Can you guess how long these took?🫣</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n93i3gxs9cgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1eip249</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>New nails🥰</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/979rib669cgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1eiolpl</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>See through nails</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eiolpl/see_through_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1eiocuh</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>new set on my naturals ☾</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiocuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1eio8g2</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>before and after….</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eio8g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1eio6aj</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>👽🛸Deep Space🛸👽</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eio6aj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1einyck</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>2 weeks progress pic!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49lz6pxd0cgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1einv6d</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Almond Nails</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1einv6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1einc1y</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ive booked into nail school! </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvz7fs7fvbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1einbik</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>my engagement nails!💍</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alr61ftavbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1eimspd</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Is this normal for my pointer and middle nail to point down?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eimspd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1eim5uy</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Am i insane or are these bad ;-;</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8jtfeqdmbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1eilwy3</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Press on’s for years, want to start my natural nail journey</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eilwy3/press_ons_for_years_want_to_start_my_natural_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1eilw7i</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Can't take my eyes off those nails!"</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d976y2u9kbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1eilv3s</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>New nailsss</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eilv3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1eiln0u</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>h0t pink toes for a h0t weekend 🥵 🌺💄</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqglp18eibgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1eiljp0</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Did my friend’s nails 🌸</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiljp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1eil5n2</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Both my thumb nails are so strong and the rest are so flaky! Anyone else struggle with inconsistency?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eil5n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1eikwfj</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>How do I get rid of the bubbles??</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc8j8k3xcbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1eikq8c</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Dashing Diva Glaze — First Attempt</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eikq8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1eikahd</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried to save her 3 times now </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eikahd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1eijn1q</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my nails done for the first time and I hate them. </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eijn1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1eijep1</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Pink French on the Vine</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eijep1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1eiilwv</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Obsessed with my Disney inspired nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h9dcus6wagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1eij75e</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First time with acrylics!💅🏻💜 (hand painted!)</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eij75e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1eiir4i</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I went for the “intentionally chipped” look. </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azmizul9xagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1eiiql5</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Just had them done, what do you think? 🧐</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oukpn7t5xagd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1eiipfx</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Went shorter and asked for some chrome! Reminds me of a beetle! 🪲</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl8qlm2xwagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1eiibck</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Latest Set</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmc2fyl1uagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1eii6w1</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>First time making my own press on nails! CC welcome</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eii6w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1eii10t</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Simple pale pink🩰</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qv8q72xragd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1eihyc5</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>I like to plan my nails beforehand, I like this design but something feels off about the left hand. What should I change?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eihyc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1eiho7r</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Nails ready for my wedding tomorrow 🥰</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em2bu1oapagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1eihn9i</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My girlfriend tried doing nail extension, she's new to doing nails in general, so I am her guinea pig </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwnu4yu3pagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1eihfcz</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Simple is nice sometimes</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4io81tinagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1eihcol</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>First time doing gel-x!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eihcol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1eigr5f</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Peel off bases</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eigr5f/peel_off_bases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1eig816</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Here are my summer nails!!!</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eig816</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1eifi48</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>How do i keep my nails healthy?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eifi48/how_do_i_keep_my_nails_healthy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1eifzdn</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Finally learned the key to at home gel nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56n2635zcagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1eifmhy</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Switched my almond for stiletto ones 🧙🏻‍♀️ </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ijo5edaagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1eifj9o</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Shades of Purple💜</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eifj9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1eifiuc</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Should I change shape?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eifiuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1eifb7y</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Last of summer 🌼</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llc09c948agd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1eif869</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>got my nails done today</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fslce9wj7agd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1eiewvs</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Anyone else obsessed with iridescent nails?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spknd9ja5agd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1eiert4</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails. What do you think? </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv1f9b7c4agd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1eie4w7</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using press ons </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eie4w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ei569p</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Is this reasonable discoloration in 48 hours?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei569p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1eidkul</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Any tips on how to avoid this? New to builder gel!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3cbvbktv9gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ei6ygu</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>BIAB vs. Rubber Base - what’s the difference?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ei6ygu/biab_vs_rubber_base_whats_the_difference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ei7n23</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>cirque bird day haul</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pfrzinik8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ei8kn2</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help guys! I need some inspo I have a nail appointment today I wanna do something fun and bright! Please leave inspo pics in comments! This my current set! </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv8ka0y8t8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1eidgza</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Getting a fill tomorrow so wanted to share the pink French tip one more time 🥺</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eidgza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1eidfcz</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Loving these short pink cuties 🌸</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eidfcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1eid8l9</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yin &amp; Yang Nails </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eid8l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ei9u88</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Is this ok? Or should I go back?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei9u88</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1eiahvu</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Can you use regular polish on top of gel?</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eiahvu/can_you_use_regular_polish_on_top_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1eibqm8</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Why do Instagram techs have such long menus?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eibqm8/why_do_instagram_techs_have_such_long_menus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1eibzw8</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of this design! Simple with a touch of black  </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mucaw7kk9gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1eicjnw</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My first ever nail!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eicjnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1eicfe5</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice needed on French mani! </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eicfe5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1eicetw</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Gel chipping</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eicetw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1eic4ho</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>august nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p9cuv1hl9gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1eibksz</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Blue days 🌥️</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wosygzih9gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1eiwq36</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>PLEASE HELP</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o87qitrcaegd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1eiw32x</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">That's the Spirit </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiw32x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1eiv5fy</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Vintage Sally Hansen Red!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag8dom3usdgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1eiph8t</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>July Mani Roundup</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiph8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1eitw1q</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Matte White</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eitw1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1eisqta</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>China Glaze For Audrey</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z80ltvt5dgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1eism38</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Weeping Willow - Mooncat</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bazxilpn4dgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1eir64y</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Word on the street (the street being Facebook) is Psilocybin by Clionadh will possibly be returning for the holidays 👀</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eir64y/word_on_the_street_the_street_being_facebook_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1eiqmnx</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>ILNP Mint Chip and Strawberry Shake</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiqmnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1eiq1uj</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Cirque Spa Water free gift</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiq1uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1eip3b4</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>About to see Justice, did a quick mani based off Cross' color scheme</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eip3b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1eiopo1</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>my first kbshimmer polish 💅</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg64vzyh6cgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1eioljm</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Death valley nails haul 💀❤️</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eioljm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1eioawe</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Some bubblegum pink to brighten your day 🌸</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eioawe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ein9ja</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🛸Deep Space🛸 </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ein9ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ein65g</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a color recommendation </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz11vmf4ubgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1eimq1n</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>By Dany Vianna - Rosewater 2.0 (PPU Rewind ‘24) 🌸</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eimq1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1eim6yh</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Too many pink polishes or not enough?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54bu689mmbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1eim5lt</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Can't stop looking at these... Valentine's Day came early! (Crystal Knockout - 25 Fly)</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eim5lt/cant_stop_looking_at_these_valentines_day_came/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1eilfhy</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>forgot how bright and summery this one is 💖</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1zu99rugbgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1eil3eg</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polished For Days - Blossom🌸 </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eil3eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1eil36h</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Look at my treasures!!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql2sxhucebgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1eikzkk</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Acid Rain</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e3dyscgidbgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1eikrt7</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>what kind of manicure won't damage long nails?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eikrt7/what_kind_of_manicure_wont_damage_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1eijtci</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Ruby by ILNP topped with Solar Unicorn Taco by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eijtci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1eijstm</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Need recs for quick dry spray to replace OPI</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eijstm/need_recs_for_quick_dry_spray_to_replace_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1eijdou</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Zombie claw</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eijdou/zombie_claw/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1eij83o</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Pleasing- Wearing crème again after a long time</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ihxn7gq0bgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1eij2fz</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>New mani ft. My cat and a slight smudge</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2amfpa6kzagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1eij19b</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are gradients so hard for me?! </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg45g26czagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1eiiqt4</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green Lovers Dream 💚💚💚 (PPU Rewind) </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiiqt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1eihxzv</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>A first: client insisted on sitting in my lap during service</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15ld00naragd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1eihtzf</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Switching back to DIY</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eihtzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1eiglfe</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shang-Chi infinity knot (MCU) nail art </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ouym8pehagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1eigdpz</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>What nail polish is used on Gwen in the luxurious MV?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uh06e2fufagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1eig8yv</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Mimic Spider during golden hour 🕷☀</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4czvgzneagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1eifc5u</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Cheap in the name not on the nails ✨</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swesjeua8agd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ei2ypj</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Palette cleanser mani for this week🌼</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei2ypj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ei2w3s</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KB Shimmer Flake Expectations &amp; Oh Matte! over black </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtq2ijbuugt51.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ehyiro</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Looking for a similar colour - Sugar</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehyiro/looking_for_a_similar_colour_sugar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ehu6bu</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Ex Nail biter - How do I look after my nails?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ehu6bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ehphp6</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help shade matching! </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ehphp6/please_help_shade_matching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1eicrdn</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>It's Nailsquatch!</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eicrdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1eib7x5</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Best toppers?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eib7x5/best_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1eialwv</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Can you use regular polish on top of gel polish?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eialwv/can_you_use_regular_polish_on_top_of_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1eiaev6</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>ILNP - Pitter Patter, Rainy Days, Starlight &amp; Thundercloud ⛈️💙🌧</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiaev6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ei8g34</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co- Cherry Blossom (PPU Rewind)</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9zi6hwsr8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ei8ees</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Note, shop for polishes at TJ Maxx more often 😍</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei8ees</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ei7oqc</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Cirque bird day haul</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arj614nyk8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1eixasc</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>This is by far my favourite nail set! Should I get them? (I'm a total Hanta Sero fan BTW.)</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/CVaIkm6pOmV/?igsh=dXFqNWd0MG04YXc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1eix9z8</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Glass-like cat eye!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eix9z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1eivw56</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>My first time doing this!!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hufykh2x0egd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1eiugbk</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Anime nails on my client</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px9ap5otldgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1eitlv8</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>What do you think of this effect and color? 🤔</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lseq0c7qddgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1eitknw</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful nails 😍 How is the combination? </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpr5g3ueddgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1eis4xx</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Total beginner, just got a “stand” thingy. Could DEFINITELY use some tips!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6357bwe0dgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1eioayd</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bkb0nx63cgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1eio1yv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>I love my job, my clients and their designs 💖💅🏻</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eio1yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1eimfbi</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>First time I did my own nails</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eimfbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1eilhwb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello, I present my designs and I like to read constructive opinions. </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eilhwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1eikm5x</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Beautiful color combination, i love how they turned out 😍</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eikm5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1eiik2o</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>What are they?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea9axeatvagd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1eihapc</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I have a (possibly) stupid question!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eihapc/i_have_a_possibly_stupid_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1eifnva</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Gummy Candy Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eifnva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1eiesjb</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails. Colourful French </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiesjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ei8vio</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Love this beautiful animal print design 😍 what do you think?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra0ulu4zv8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ei8h3q</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like the freehand style? I am in love </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyk5wf7fs8gd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ei88mr</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Story telling nail art, a story about Duke Bunny and his wife, the Duchess </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei88mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ei6jfk</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>van gogh nails! done by me</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei6jfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ei66d2</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Who remembers Recess??</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ei66d2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug  4 08:08:17 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_04.xlsx
+++ b/data/2024_08_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1185"/>
+  <dimension ref="A1:C1360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20578,6 +20578,2982 @@
         </is>
       </c>
     </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ejph1q</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">House of Hades + Moon Dust and Midnight Rider. </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7p4s3jt8mlgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ejozoz</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>I’m redoing my nails tomorrow and wanted to show these off even tho they’re so messed up from my job 🥲🥲🥲💘 rip to these clown nails hahaha</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9p4yg3kglgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ejokaz</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>nail is growing flat at the end ?</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejokaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ejo5ea</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Working a “denim and diamonds” themed event, so went with high power sparkle.</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpigy2ym6lgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ejnv57</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time gel nails with extension </t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ei00sr683lgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ejnql1</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>My first ever jujutsu Kaisen set! I’ve been wanting to do one for the longest time but finally I got a commission. I’m super proud of how I did on this</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejnql1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ejnn9o</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Pinky red sparkles 💕</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejnn9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ejmfco</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Lilac Ombré Coffin</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejmfco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ejlu4j</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>End of Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejlu4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ejln3o</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Regular acetone for gel polish removal? + your advice and recommendations!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejln3o/regular_acetone_for_gel_polish_removal_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ejjq0w</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie! </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejjq0w/newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ejkpkp</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>What do you think of this design with stickers?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw5ulcqw6kgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ejl9ap</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Princess Nails!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejl9ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ejl7qf</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>💙👁️💙</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbmwo0gobkgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ejl0ct</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Am I the only one who feel like a lot of nail salons just don't do shit right?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejl0ct/am_i_the_only_one_who_feel_like_a_lot_of_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ejky6n</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Formal Lumpy Space</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejky6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ejkvrn</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>seashell nails🐚</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znq6desj8kgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ejkr6l</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Shaped and painted my own natural nails for the first time. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejkr6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ejknup</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>New Blue Chrome Nails 🩵 🫧</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc0fjoyg6kgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ej83cl</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Bumped my nail and i cracked in the middle, what do i do?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej83cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ejdnj1</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Most natural looking option for manicures?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejdnj1/most_natural_looking_option_for_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ejdvnh</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>As a hobbyist, what are your boundaries for doing friends/family’s nails?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejdvnh/as_a_hobbyist_what_are_your_boundaries_for_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1eje7yx</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>i have found my people. seeking advice!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eje7yx/i_have_found_my_people_seeking_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1eji8qc</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>New nail tech. Obsessed!</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb6zn9p1kjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ejjhrv</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Nail wrap haul! Got carried away, and now I don’t know which set to start with! 😭</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1vybiyevjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ejk6e9</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time trying stiletto </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejk6e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ejjc0u</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best way to keep natural nails strong </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejjc0u/best_way_to_keep_natural_nails_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ejjbpg</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejjbpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ejiy3w</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Is there any way to fix this</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejiy3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ejgt19</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Cracked dip powder. Will I need a new full set?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejgt19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ejhw4p</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Deep nail split help</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdjb9npygjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ejiagk</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coraline Nails </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erb2mfkhkjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1eji8hv</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Why do nail salons add extensions to the tip of the nail?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eji8hv/why_do_nail_salons_add_extensions_to_the_tip_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1eji39l</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kirby set </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo7kqo4oijgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ejeywi</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Did my nails!!</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejeywi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ejfsn7</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Quick dry and nail strengthening polish?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejfsn7/quick_dry_and_nail_strengthening_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ejg87z</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>I’ve been getting my nails done for years and my tech is just the best so I wanted to share some of my fave sets over the years 🫶🏼💅</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejg87z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ejg4g1</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>What can use for bendy nails?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejg4g1/what_can_use_for_bendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ejfyp7</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>New selfmade summer nails ☀️</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8me45srq0jgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ejfuxp</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic french manicure </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ko6x053wzigd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ejfr5r</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hella Handmade Creations | July 2024 - Walk on the wild side</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z381etf0zigd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ejfgd3</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my nails done for the first time ever at age 34, what do you think of the style? </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rqr0uwmwigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ejfcag</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Clear vs frosted- what's the difference?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgflwodrvigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ejf32l</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Classic Almond French 🤩</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d60w65ptigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ejewyj</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Watched 1 YouTube tutorial and this is my 1st try! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejewyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ejbekh</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In need of advice </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejbekh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ejch7t</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Low effort 😭?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejch7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ejchaj</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanting to do glitter jelly nails.. can I use resin pigment to add to clear polish? </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejchaj/wanting_to_do_glitter_jelly_nails_can_i_use_resin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1eje8hi</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate my nails </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0lsolyomigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1eje5j9</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there anything I can do? Or should I go back to the salon ? </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cybvgjy1migd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ejdybb</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Potential wedding nails!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejdybb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ejds2x</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Started my own gel journey</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drdon4z4jigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1ejdmnp</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Pointed red tips. I feel like such a baddie in these</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejdmnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1ejdi4t</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>French tips but make it ✨sparkly✨</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejdi4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ejd7hm</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">House of Hades and Moon dust. YES PLEASE. </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejd7hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ejczq6</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Current status of nails…sigh..help! </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejczq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ejc7pk</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>First time applying biab</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejc7pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ejbine</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>A new enemy has arrived… feat. Invisalign</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhn55wb81igd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ej85u7</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Press on glue on Beetles tips?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej85u7/press_on_glue_on_beetles_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ejbdww</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Got extra sparkly today ✨💖</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udxnoal80igd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ejb1ww</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Full summer mode engaged</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lluyia5nxhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ejb0pi</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>something simple and cute</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn2ycg5dxhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ejaxxb</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails normal for a 19y.o. male? They seem a bit juvenile to me at times. </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ejaxxb/are_my_nails_normal_for_a_19yo_male_they_seem_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ejasxv</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Broken heart</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4szbkx7nvhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ejafm9</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Gave myself a mani for the first time in 10+ years</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejafm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ejaejo</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set for summer </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejaejo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ejae86</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Fierce Mojo</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejae86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ej9wop</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink nails </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rl1oa9sohgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ej9f2s</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Electric nail files recommendations? Where do I even start?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej9f2s/electric_nail_files_recommendations_where_do_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ej9ang</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Just trying out some things</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej9ang</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ej92eh</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girly pink nails </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej92eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ej8vrq</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>I’m so proud of these</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww2u9lt9hhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ej8tgn</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4do7otsghgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ej7qqz</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like my nails look how fizzy water tastes </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hawaewg49hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1ej7g4f</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting gel off WITHOUT scraping? </t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej7g4f/getting_gel_off_without_scraping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1ej6y4f</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>tips on color choice to cover up discoloration on nails?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej6y4f/tips_on_color_choice_to_cover_up_discoloration_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1ej6sa9</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>What color should I pick?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90a8ve632hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1ej744w</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Cow Abduction!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3io4f2jg4hgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1ej70fc</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Blue summer set</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej70fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1ej6ueq</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>First time asking for a design definitely not disappointed</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgfreyji2hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1ej6kvf</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Design in red wine with a touch of shine ✨</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txfehu0k0hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1ej5mjq</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time salon questions </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej5mjq/first_time_salon_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1ej6fks</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Blue nails 💙</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7xuzmrfzggd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1ej65ir</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did my own nails for the first time! How did I do? </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej65ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1ej652l</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Transitional set 🤎natural nails… I’m in love 😍 </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej652l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1ej64gx</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>i did them myself and just wanted to show these off 🫶</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej64gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ej635p</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>my post was removed for improperly hexing u all here’s my coral nubs again 🦩🤌🏼🤏🏼</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej635p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1ej5xca</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lavender milk nails </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c75ln3tjvggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1ej21gy</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Black UV gel polish is slightly dentable and I’ve troubleshooted the hell out of this</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ej21gy/black_uv_gel_polish_is_slightly_dentable_and_ive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1ej2b79</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>This group inspired me to put on nail polish (which I rarely do)!</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zler2fta1ggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1ej53ip</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went back to a nude, I love getting colourful french tips! </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej53ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1ej3ezn</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Nail tech did me right!!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jqdihbbbggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ej3bak</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing! And who doesn’t love Stitch?! 💙💖</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej3bak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ej2vag</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Whale looks like it’s almost time for a new manicure</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aptmvsh6ggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ej2o9h</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>I’m so proud of myself</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9btiicts4ggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ej15oh</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Does anybody else take a break after doing builder gel and you almost don't want to paint them because they look so nice already?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdm80413qfgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ej0tem</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Love them but going short anyway</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5ya958jmfgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ej0ssq</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>At the end of the day I will always choose nude nails (with a twist). Took me ages to do it on myself</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej0ssq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ej07y9</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Lifted gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej07y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1eiz439</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail correction </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eiz439</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ejol73</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Jojoba Oil Recommendations</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejol73/jojoba_oil_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ejohlq</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Intense gratitude! </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejohlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ejnnmp</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Looking for weird/ugly crème colors!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejnnmp/looking_for_weirdugly_crème_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ejnk83</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>ordering ppu when i'm moving (and don't know my new mailing address)</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejnk83/ordering_ppu_when_im_moving_and_dont_know_my_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ejnj8s</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you like to do two-color manis? In need of new ideas! </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejnj8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ejn6s3</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Press ons with medium to long natural nails?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbqirc3ovkgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ejmzbc</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Lumen Myths &amp; Monsters: Cthulhu (mystery spoilers)</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejmzbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ejkh4d</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Acetone on that deeply broken nail be like</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejkh4d/acetone_on_that_deeply_broken_nail_be_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ejkeza</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>What do I do with these wide nailbeds?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejkeza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ejkbop</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Testing a Look</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u32yvs073kgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ejkaqe</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are healthy nails with long term gel possible? </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejkaqe/are_healthy_nails_with_long_term_gel_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ejj37u</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Substitue for Sally Hansen Flash?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1hz0jkkrjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ejijw5</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Help!! 48 hours of wear</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzi4xpdumjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ejia2m</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I cannot steer a lime: An Experiment </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejia2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ejhs4b</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Sparkly goodness ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejhs4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ejgryr</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>When you take a break from (normal) polish, do you put a nail treatment on your nails? Like a soothing treatment/nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejgryr/when_you_take_a_break_from_normal_polish_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ejgn09</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>I think I need help applying colours. Any constructive ideas are really appreciated thank you.</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejgn09/i_think_i_need_help_applying_colours_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ejgext</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Thoughts on Jojoba Oil?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejgext/thoughts_on_jojoba_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1ejg6km</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Halloween vibes? 🎃</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejg6km</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1ejg23b</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a shade match to this Lego piece?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw6amlei1jgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1ejfsun</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Can you guys help me identify this shade of pink and why I don’t like it on myself?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejfsun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1ejfph4</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Hella Handmade Creations | July 2024 - Walk on the wild side</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejfph4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ejfo6l</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>I need to share my donut nails 🍩</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejfo6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ejf8ib</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>A PB&amp;J type vibe!! I’m a beginner so not super good yet 😊</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejf8ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ejedwr</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Nail salon employee ruined my new sandals. What is fair?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejedwr/nail_salon_employee_ruined_my_new_sandals_what_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1eje0fo</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Is there a nail polish with a iridescent/shimmer magenta shine? Kinda like the pics below but nail lacquer/normal polish</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eje0fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ejdymj</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Last time I didn't have a glitter smoother so the flakes didn't show as well, but now I do (In the garden flakie mystery, Kathleen and co)</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpwxlkfjkigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ejdfzt</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>My LA Colors obsession continues</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejdfzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ejd4i6</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with builder gel lifting! </t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejd4i6/help_with_builder_gel_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ejcwd5</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>How do I clean my nail tools?</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejcwd5/how_do_i_clean_my_nail_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ejclvp</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Shake Your Shamrock - Dreamland Lacquer</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9liyezxu9igd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ejcaw4</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Illusionist on shorties🥀</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4g8hxisb7igd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ejc2iz</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday mani 🎂 </t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejc2iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ejbfyk</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>I put on a shirt and went outside to take these photos ☀️</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejbfyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ejb2jn</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>she’s so Julia 💚🍏</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfd38zbsxhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ejabxa</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Fierce Mojo</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejabxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ejaaxa</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>How long does it take you to paint your nails on average?</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ejaaxa/how_long_does_it_take_you_to_paint_your_nails_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ej9uk8</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>[Nail Help] I've had problems with my nails peeling for honestly the last 25 years. I try to hydrate with Vaseline but it doesn't seem to improve. What should I be doing to prevent these flaky nail areas?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t49ln628nhgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1ej9ud4</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Penny talk </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej9ud4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ej975a</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej975a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1ej94i9</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Sassy sauce hexcellent</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej94i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ej8p65</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>my new favorite polish 🤩</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2j1i6vaufhgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ej7wdi</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Dotted daisies</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej7wdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ej7v2e</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Neon blue for August</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p27th5z9hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ej6xc6</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Help finding a gel dupe for the sheer 'sea glass' type polish here?</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ej6xc6/help_finding_a_gel_dupe_for_the_sheer_sea_glass/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ej62qs</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass Ceiling is a FANTASTIC topper </t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1lwk5dqwggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ej5yyv</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings Shorties</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obwx53mwvggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ej5ygo</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails tearing </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej5ygo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ej53gl</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Xu Xialing inspired nail art (mcu) </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynewjcq6pggd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ej44gr</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Any nail art ideas or nail polish recommendations that would fit this dress?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej44gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1ej11j3</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What I wore in July</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej11j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1eizmdi</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Nail popped right off (normal laquer). Is this a sign that the base coat is bad?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f800tnkz8fgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1ejpmc0</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Just got into doing nail art in June! I don’t use any acrylic/gel, just the regular stuff plus glue</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejpmc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1ejnj4r</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Ocean beach type nail🌊🌊</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejnj4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ejndyq</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Playing with cat eye gels</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejndyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ejl9xr</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time doing nails with gems &amp; using gel products I bought in Seoul
+</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ejl9xr/my_first_time_doing_nails_with_gems_using_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1ejkdan</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>different colors of bases, on top of all other different shiny powders, once all the nail bases are made, the different shapes are created with gel. in some larger and in other smaller amounts. For the finer lines, some diamond or piece was added in the center and we added pigment to the gel 😇</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbt0ibxm3kgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ejk766</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time trying stiletto </t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejk766</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1ejh82e</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Love love love</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiutztu8bjgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ejgv3m</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Long or short?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejgv3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ejgoop</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>cherries 🍒 and checkers 🏁!</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejgoop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1ejfrpv</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Today's Project 🤪</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejfrpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1ejfo6n</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Is there an alternative for transfer gel?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ejfo6n/is_there_an_alternative_for_transfer_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1eje026</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>The Beatles</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eje026</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ejdnlz</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Support the mix of techniques?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1do55qj5iigd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ejdjnd</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Nail Art</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pqug0yr0higd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ejctja</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY of my latest set </t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejctja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1ejbh3m</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today's design, I want to clarify that the plush is foldable. </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ejbh3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ej8wuw</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Summer vibes with a beautiful dragonfly ✨</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivy4isxhhhgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1ej8s9n</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Mushroom Nail Art</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy3mfzihghgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1ej6w5x</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>What do you think about this</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pv64ix7b2hgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1ej6vr5</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Blue summer set</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej6vr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ej6pyk</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Which set to finish first?</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vieiwzm1hgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ej3a7k</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>My nail tech is so amazing!! And who doesn’t love Stitch?! 💙💖</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej3a7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1ej0vao</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>different gel-free bases and styles, simulating precious stones 👀😁</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ej0vao</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>